<commit_message>
Updated based on latest PIO
</commit_message>
<xml_diff>
--- a/COVID-Malabon-DS.xlsx
+++ b/COVID-Malabon-DS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kderaco\Documents\GitHub\malabon-covid19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A04F65-549A-46C6-99F4-2F2064453CE9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812B6C9D-4A30-4736-BFE5-FEE09DD40E65}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="10845" activeTab="1" xr2:uid="{75DE67D3-5672-4499-AF5E-02B4779C1C44}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="109">
   <si>
     <t>Barangays</t>
   </si>
@@ -359,6 +359,24 @@
   </si>
   <si>
     <t>Tondo General Hospital</t>
+  </si>
+  <si>
+    <t>MALCP-23</t>
+  </si>
+  <si>
+    <t>MALCP-24</t>
+  </si>
+  <si>
+    <t>MALCP-25</t>
+  </si>
+  <si>
+    <t>MALCP-26</t>
+  </si>
+  <si>
+    <t>MALCP-27</t>
+  </si>
+  <si>
+    <t>--</t>
   </si>
 </sst>
 </file>
@@ -447,7 +465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -497,6 +515,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1322,10 +1341,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{235D48F9-A32C-4C88-8D8A-9730C606D5F1}">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -2010,38 +2029,150 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C24" s="19"/>
-      <c r="D24" s="4" t="e">
+      <c r="A24" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="20">
+        <v>43935</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="4" t="str">
         <f>VLOOKUP(C24,Barangay!$A$2:$C$22,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E24" s="4" t="e">
+        <v>MAL-BGY-017</v>
+      </c>
+      <c r="E24" s="4" t="str">
         <f>VLOOKUP(C24,Barangay!$A$2:$C$22,2,0)</f>
-        <v>#N/A</v>
+        <v>District 2</v>
+      </c>
+      <c r="G24" s="4">
+        <v>33</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I24" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D25" s="4" t="e">
+      <c r="A25" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="20">
+        <v>43935</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="4" t="str">
         <f>VLOOKUP(C25,Barangay!$A$2:$C$22,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E25" s="4" t="e">
+        <v>MAL-BGY-007</v>
+      </c>
+      <c r="E25" s="4" t="str">
         <f>VLOOKUP(C25,Barangay!$A$2:$C$22,2,0)</f>
-        <v>#N/A</v>
+        <v>District 1</v>
+      </c>
+      <c r="G25" s="4">
+        <v>50</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I25" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D26" s="4" t="e">
+      <c r="A26" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="20">
+        <v>43935</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="4" t="str">
         <f>VLOOKUP(C26,Barangay!$A$2:$C$22,3,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E26" s="4" t="e">
+        <v>MAL-BGY-019</v>
+      </c>
+      <c r="E26" s="4" t="str">
         <f>VLOOKUP(C26,Barangay!$A$2:$C$22,2,0)</f>
-        <v>#N/A</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C27" s="19"/>
+        <v>District 2</v>
+      </c>
+      <c r="G26" s="4">
+        <v>53</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I26" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27" s="21">
+        <v>43935</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="15" t="str">
+        <f>VLOOKUP(C27,Barangay!$A$2:$C$22,3,0)</f>
+        <v>MAL-BGY-019</v>
+      </c>
+      <c r="E27" s="15" t="str">
+        <f>VLOOKUP(C27,Barangay!$A$2:$C$22,2,0)</f>
+        <v>District 2</v>
+      </c>
+      <c r="G27" s="15">
+        <v>60</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="I27" s="15">
+        <v>1</v>
+      </c>
+      <c r="J27" s="15">
+        <v>1</v>
+      </c>
+      <c r="K27" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="20">
+        <v>43935</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="4" t="str">
+        <f>VLOOKUP(C28,Barangay!$A$2:$C$22,3,0)</f>
+        <v>MAL-BGY-021</v>
+      </c>
+      <c r="E28" s="4" t="str">
+        <f>VLOOKUP(C28,Barangay!$A$2:$C$22,2,0)</f>
+        <v>District 2</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I28" s="4">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -2211,7 +2342,7 @@
       </c>
       <c r="D8" s="4">
         <f>SUMIF('Confirmed Cases'!$C$2:$C$100,'Summary-District'!B8,'Confirmed Cases'!$I$2:$I$100)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="4">
         <f>SUMIF('Confirmed Cases'!$C$2:$C$100,'Summary-District'!B8,'Confirmed Cases'!$J$2:$J$100)</f>
@@ -2401,7 +2532,7 @@
       </c>
       <c r="D18" s="4">
         <f>SUMIF('Confirmed Cases'!$C$2:$C$100,'Summary-District'!B18,'Confirmed Cases'!$I$2:$I$100)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="4">
         <f>SUMIF('Confirmed Cases'!$C$2:$C$100,'Summary-District'!B18,'Confirmed Cases'!$J$2:$J$100)</f>
@@ -2439,11 +2570,11 @@
       </c>
       <c r="D20" s="4">
         <f>SUMIF('Confirmed Cases'!$C$2:$C$100,'Summary-District'!B20,'Confirmed Cases'!$I$2:$I$100)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E20" s="4">
         <f>SUMIF('Confirmed Cases'!$C$2:$C$100,'Summary-District'!B20,'Confirmed Cases'!$J$2:$J$100)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -2477,7 +2608,7 @@
       </c>
       <c r="D22" s="4">
         <f>SUMIF('Confirmed Cases'!$C$2:$C$100,'Summary-District'!B22,'Confirmed Cases'!$I$2:$I$100)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="4">
         <f>SUMIF('Confirmed Cases'!$C$2:$C$100,'Summary-District'!B22,'Confirmed Cases'!$J$2:$J$100)</f>
@@ -2786,11 +2917,11 @@
       </c>
       <c r="B22" s="1">
         <f>COUNTIF('Confirmed Cases'!$B$2:$B$100,'Summary per Day'!A22)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C22" s="24">
         <f>SUMPRODUCT(--('Confirmed Cases'!$B$2:$B$100='Summary per Day'!A22),'Confirmed Cases'!$J$2:$J$100)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -3004,15 +3135,15 @@
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="23">
         <f ca="1">NOW()</f>
-        <v>43934.517519444445</v>
+        <v>43935.855562731478</v>
       </c>
       <c r="B73" s="1">
         <f>SUM('Confirmed Cases'!I2:I100)</f>
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C73" s="24">
         <f>SUM('Confirmed Cases'!J2:J100)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -3054,15 +3185,15 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <f ca="1">NOW()</f>
-        <v>43934.517519444445</v>
+        <v>43935.855562731478</v>
       </c>
       <c r="B2" s="1">
         <f>SUM('Confirmed Cases'!I2:I100)</f>
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1">
         <f>SUM('Confirmed Cases'!J2:J100)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>

</xml_diff>